<commit_message>
Merged drought and county dataframes.
</commit_message>
<xml_diff>
--- a/Data cleanup procedure example.xlsx
+++ b/Data cleanup procedure example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdelc\BootCamp\Repositories\Project1_Droughts_USA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087E6527-CC4D-4C82-A01D-BD8B1EB45856}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5171C6-4E29-4C59-B869-18905C3D91A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2550" yWindow="2595" windowWidth="27165" windowHeight="15270" xr2:uid="{81D7ECD8-0384-494B-B197-BEB46A44B807}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="8">
   <si>
     <t>None</t>
   </si>
@@ -409,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A9CF73-9590-4588-BC23-98A7088C3BEB}">
-  <dimension ref="C14:J18"/>
+  <dimension ref="C14:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,6 +517,106 @@
         <v>100</v>
       </c>
     </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" t="s">
+        <v>5</v>
+      </c>
+      <c r="J24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>100</v>
+      </c>
+      <c r="E25">
+        <v>100</v>
+      </c>
+      <c r="F25">
+        <v>100</v>
+      </c>
+      <c r="G25">
+        <v>100</v>
+      </c>
+      <c r="H25">
+        <v>74.5</v>
+      </c>
+      <c r="J25">
+        <f>100-C25</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" t="s">
+        <v>5</v>
+      </c>
+      <c r="J27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <f>C25</f>
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <f>D25-E25</f>
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <f>E25-F25</f>
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <f>F25-G25</f>
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <f>G25-H25</f>
+        <v>25.5</v>
+      </c>
+      <c r="H28">
+        <f>H25</f>
+        <v>74.5</v>
+      </c>
+      <c r="J28">
+        <f>SUM(C28:H28)</f>
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>